<commit_message>
Add Jan GTFS data and insert some data into the draft
</commit_message>
<xml_diff>
--- a/doc/APC-GTFS.xlsx
+++ b/doc/APC-GTFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ro2_apc" sheetId="1" state="hidden" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <sheet name="b_2_apc" sheetId="7" state="hidden" r:id="rId14"/>
     <sheet name="b_2_gtfs" sheetId="8" state="hidden" r:id="rId15"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId16"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">hour_merge!#REF!</definedName>
   </definedNames>
@@ -1979,42 +1976,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>month_merge!$B$2:$B$12</c:f>
+              <c:f>month_merge!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.3888333333333334</c:v>
+                  <c:v>3.9231666666666665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1751666666666667</c:v>
+                  <c:v>3.4316666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5666666666666669</c:v>
+                  <c:v>3.5215000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9994999999999998</c:v>
+                  <c:v>3.8800000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2701666666666669</c:v>
+                  <c:v>4.1795</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4356666666666666</c:v>
+                  <c:v>3.5985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3448333333333329</c:v>
+                  <c:v>4.3491666666666662</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0766666666666667</c:v>
+                  <c:v>4.153833333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1661666666666664</c:v>
+                  <c:v>4.1875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1091666666666669</c:v>
+                  <c:v>3.3935000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2314999999999996</c:v>
+                  <c:v>2.9376666666666664</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.3136666666666668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,42 +2095,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>month_merge!$C$2:$C$12</c:f>
+              <c:f>month_merge!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>6.58</c:v>
+                  <c:v>7.26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.34</c:v>
+                  <c:v>6.660000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.98</c:v>
+                  <c:v>6.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.66</c:v>
+                  <c:v>7.2700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.2</c:v>
+                  <c:v>7.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.78</c:v>
+                  <c:v>6.87</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.01</c:v>
+                  <c:v>8.23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.74</c:v>
+                  <c:v>8.06</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9600000000000009</c:v>
+                  <c:v>8.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.0500000000000007</c:v>
+                  <c:v>6.7299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.78</c:v>
+                  <c:v>5.82</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2221,31 +2224,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="3">
-                  <c:v>4.9178333333333333</c:v>
+                  <c:v>4.4283333333333328</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9084999999999996</c:v>
+                  <c:v>4.9543333333333335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.2545000000000002</c:v>
+                  <c:v>4.3261666666666665</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0679999999999996</c:v>
+                  <c:v>5.0908333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6955</c:v>
+                  <c:v>4.8711666666666664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.7540000000000004</c:v>
+                  <c:v>4.782</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.6979999999999995</c:v>
+                  <c:v>5.1733333333333329</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.1671666666666667</c:v>
+                  <c:v>3.5665</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7395</c:v>
+                  <c:v>3.9063333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2336,31 +2339,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="3">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>8.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.24</c:v>
+                  <c:v>9.2200000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.15</c:v>
+                  <c:v>8.19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.27</c:v>
+                  <c:v>9.5500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.8500000000000005</c:v>
+                  <c:v>9.34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0399999999999991</c:v>
+                  <c:v>9.1800000000000015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.1300000000000008</c:v>
+                  <c:v>8.73</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.34</c:v>
+                  <c:v>7.0000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.7799999999999994</c:v>
+                  <c:v>7.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2439,6 +2442,7 @@
         <c:axId val="450161992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4288,16 +4292,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4319,489 +4323,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="all"/>
-      <sheetName val="all_distribution"/>
-      <sheetName val="dedicated_timeseries"/>
-      <sheetName val="dedicated_diff_compare_method"/>
-      <sheetName val="dedicated_diff_direct_method"/>
-      <sheetName val="dedicated_a_and_b_direct_method"/>
-      <sheetName val="dedicated_nov"/>
-      <sheetName val="dedicated_a_and_b"/>
-      <sheetName val="dedicated_a_b_ttp"/>
-      <sheetName val="dedicated_transfer_risk"/>
-      <sheetName val="dedicated_tr"/>
-      <sheetName val="ded_tr_plot"/>
-      <sheetName val="month"/>
-      <sheetName val="hour"/>
-      <sheetName val="weekday"/>
-      <sheetName val="rain"/>
-      <sheetName val="football"/>
-      <sheetName val="attp_diff_distribution"/>
-      <sheetName val="attp_diff_distribution_log"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Average Total Time Penalty (minutes)</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Transfer Risk (%)</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Feb</v>
-          </cell>
-          <cell r="B2">
-            <v>3.3888333333333334</v>
-          </cell>
-          <cell r="C2">
-            <v>6.58</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Mar</v>
-          </cell>
-          <cell r="B3">
-            <v>3.1751666666666667</v>
-          </cell>
-          <cell r="C3">
-            <v>6.34</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Apr</v>
-          </cell>
-          <cell r="B4">
-            <v>3.5666666666666669</v>
-          </cell>
-          <cell r="C4">
-            <v>6.98</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>May</v>
-          </cell>
-          <cell r="B5">
-            <v>3.9994999999999998</v>
-          </cell>
-          <cell r="C5">
-            <v>7.66</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Jun</v>
-          </cell>
-          <cell r="B6">
-            <v>3.2701666666666669</v>
-          </cell>
-          <cell r="C6">
-            <v>6.2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Jul</v>
-          </cell>
-          <cell r="B7">
-            <v>3.4356666666666666</v>
-          </cell>
-          <cell r="C7">
-            <v>6.78</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Aug</v>
-          </cell>
-          <cell r="B8">
-            <v>5.3448333333333329</v>
-          </cell>
-          <cell r="C8">
-            <v>10.01</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Sep</v>
-          </cell>
-          <cell r="B9">
-            <v>3.0766666666666667</v>
-          </cell>
-          <cell r="C9">
-            <v>5.74</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Oct</v>
-          </cell>
-          <cell r="B10">
-            <v>4.1661666666666664</v>
-          </cell>
-          <cell r="C10">
-            <v>7.9600000000000009</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Nov</v>
-          </cell>
-          <cell r="B11">
-            <v>4.1091666666666669</v>
-          </cell>
-          <cell r="C11">
-            <v>8.0500000000000007</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Dec</v>
-          </cell>
-          <cell r="B12">
-            <v>2.2314999999999996</v>
-          </cell>
-          <cell r="C12">
-            <v>4.78</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Average Total Time Penalty (minutes)</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Transfer Risk (%)</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>0.20833333333333334</v>
-          </cell>
-          <cell r="B2">
-            <v>1.8496666666666668</v>
-          </cell>
-          <cell r="C2">
-            <v>3.17</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>0.25</v>
-          </cell>
-          <cell r="B3">
-            <v>2.3556666666666666</v>
-          </cell>
-          <cell r="C3">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>0.29166666666666702</v>
-          </cell>
-          <cell r="B4">
-            <v>2.9855</v>
-          </cell>
-          <cell r="C4">
-            <v>6.47</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>0.33333333333333298</v>
-          </cell>
-          <cell r="B5">
-            <v>3.3673333333333333</v>
-          </cell>
-          <cell r="C5">
-            <v>6.94</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>0.375</v>
-          </cell>
-          <cell r="B6">
-            <v>3.2633333333333336</v>
-          </cell>
-          <cell r="C6">
-            <v>6.49</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>0.41666666666666702</v>
-          </cell>
-          <cell r="B7">
-            <v>3.1390000000000002</v>
-          </cell>
-          <cell r="C7">
-            <v>5.99</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>0.45833333333333298</v>
-          </cell>
-          <cell r="B8">
-            <v>3.3028333333333331</v>
-          </cell>
-          <cell r="C8">
-            <v>6.370000000000001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>0.5</v>
-          </cell>
-          <cell r="B9">
-            <v>3.4863333333333335</v>
-          </cell>
-          <cell r="C9">
-            <v>6.93</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>0.54166666666666696</v>
-          </cell>
-          <cell r="B10">
-            <v>3.5451666666666668</v>
-          </cell>
-          <cell r="C10">
-            <v>7.1400000000000006</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>0.58333333333333304</v>
-          </cell>
-          <cell r="B11">
-            <v>4.2473333333333336</v>
-          </cell>
-          <cell r="C11">
-            <v>7.68</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>0.625</v>
-          </cell>
-          <cell r="B12">
-            <v>4.5409999999999995</v>
-          </cell>
-          <cell r="C12">
-            <v>8.48</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>0.66666666666666696</v>
-          </cell>
-          <cell r="B13">
-            <v>5.1028333333333338</v>
-          </cell>
-          <cell r="C13">
-            <v>9.41</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>0.70833333333333304</v>
-          </cell>
-          <cell r="B14">
-            <v>5.1710000000000003</v>
-          </cell>
-          <cell r="C14">
-            <v>10.15</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>0.75</v>
-          </cell>
-          <cell r="B15">
-            <v>4.5486666666666666</v>
-          </cell>
-          <cell r="C15">
-            <v>9.1800000000000015</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>0.79166666666666696</v>
-          </cell>
-          <cell r="B16">
-            <v>3.846166666666667</v>
-          </cell>
-          <cell r="C16">
-            <v>7.4399999999999995</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>0.83333333333333304</v>
-          </cell>
-          <cell r="B17">
-            <v>3.7611666666666665</v>
-          </cell>
-          <cell r="C17">
-            <v>6.08</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>0.875</v>
-          </cell>
-          <cell r="B18">
-            <v>3.9689999999999999</v>
-          </cell>
-          <cell r="C18">
-            <v>5.7700000000000005</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>0.91666666666666696</v>
-          </cell>
-          <cell r="B19">
-            <v>4.4671666666666665</v>
-          </cell>
-          <cell r="C19">
-            <v>6.1</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>0.95833333333333304</v>
-          </cell>
-          <cell r="B20">
-            <v>4.6860000000000008</v>
-          </cell>
-          <cell r="C20">
-            <v>6.5600000000000005</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="14">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Average Total Time Penalty (minutes)</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Transfer Risk (%)</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Mon</v>
-          </cell>
-          <cell r="B2">
-            <v>3.4506666666666663</v>
-          </cell>
-          <cell r="C2">
-            <v>6.7299999999999995</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Tue</v>
-          </cell>
-          <cell r="B3">
-            <v>3.7636666666666665</v>
-          </cell>
-          <cell r="C3">
-            <v>7.24</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Wed</v>
-          </cell>
-          <cell r="B4">
-            <v>3.8285</v>
-          </cell>
-          <cell r="C4">
-            <v>7.28</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Thu</v>
-          </cell>
-          <cell r="B5">
-            <v>3.9910000000000001</v>
-          </cell>
-          <cell r="C5">
-            <v>7.5600000000000005</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Fri</v>
-          </cell>
-          <cell r="B6">
-            <v>4.2840000000000007</v>
-          </cell>
-          <cell r="C6">
-            <v>8.129999999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Sat</v>
-          </cell>
-          <cell r="B7">
-            <v>3.5513333333333335</v>
-          </cell>
-          <cell r="C7">
-            <v>6.8900000000000006</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Sun</v>
-          </cell>
-          <cell r="B8">
-            <v>3.1508333333333334</v>
-          </cell>
-          <cell r="C8">
-            <v>5.81</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10676,7 +10197,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10715,16 +10236,16 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>3.3888333333333334</v>
+        <v>3.9231666666666665</v>
       </c>
       <c r="C2">
-        <v>6.58</v>
+        <v>7.26</v>
       </c>
       <c r="D2">
         <v>1006</v>
       </c>
       <c r="E2">
-        <v>262099</v>
+        <v>7020569</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -10732,16 +10253,16 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>3.1751666666666667</v>
+        <v>3.4316666666666666</v>
       </c>
       <c r="C3">
-        <v>6.34</v>
+        <v>6.660000000000001</v>
       </c>
       <c r="D3">
         <v>1006</v>
       </c>
       <c r="E3">
-        <v>183887</v>
+        <v>7375952</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -10749,16 +10270,16 @@
         <v>21</v>
       </c>
       <c r="B4">
-        <v>3.5666666666666669</v>
+        <v>3.5215000000000001</v>
       </c>
       <c r="C4">
-        <v>6.98</v>
+        <v>6.8000000000000007</v>
       </c>
       <c r="D4">
         <v>1008</v>
       </c>
       <c r="E4">
-        <v>263099</v>
+        <v>7254681</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -10766,31 +10287,31 @@
         <v>22</v>
       </c>
       <c r="B5">
-        <v>3.9994999999999998</v>
+        <v>3.8800000000000003</v>
       </c>
       <c r="C5">
-        <v>7.66</v>
+        <v>7.2700000000000005</v>
       </c>
       <c r="D5">
         <v>1030</v>
       </c>
       <c r="E5">
-        <v>260352</v>
+        <v>7044096</v>
       </c>
       <c r="G5">
         <v>5</v>
       </c>
       <c r="H5">
-        <v>4.9178333333333333</v>
+        <v>4.4283333333333328</v>
       </c>
       <c r="I5">
-        <v>9.1999999999999993</v>
+        <v>8.24</v>
       </c>
       <c r="J5">
         <v>1029</v>
       </c>
       <c r="K5">
-        <v>260123</v>
+        <v>5767481</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -10798,31 +10319,31 @@
         <v>23</v>
       </c>
       <c r="B6">
-        <v>3.2701666666666669</v>
+        <v>4.1795</v>
       </c>
       <c r="C6">
-        <v>6.2</v>
+        <v>7.82</v>
       </c>
       <c r="D6">
         <v>1029</v>
       </c>
       <c r="E6">
-        <v>234404</v>
+        <v>7529082</v>
       </c>
       <c r="G6">
         <v>6</v>
       </c>
       <c r="H6">
-        <v>3.9084999999999996</v>
+        <v>4.9543333333333335</v>
       </c>
       <c r="I6">
-        <v>7.24</v>
+        <v>9.2200000000000006</v>
       </c>
       <c r="J6">
         <v>1029</v>
       </c>
       <c r="K6">
-        <v>234265</v>
+        <v>7523571</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -10830,31 +10351,31 @@
         <v>24</v>
       </c>
       <c r="B7">
-        <v>3.4356666666666666</v>
+        <v>3.5985</v>
       </c>
       <c r="C7">
-        <v>6.78</v>
+        <v>6.87</v>
       </c>
       <c r="D7">
         <v>1025</v>
       </c>
       <c r="E7">
-        <v>255518</v>
+        <v>6735771</v>
       </c>
       <c r="G7">
         <v>7</v>
       </c>
       <c r="H7">
-        <v>4.2545000000000002</v>
+        <v>4.3261666666666665</v>
       </c>
       <c r="I7">
-        <v>8.15</v>
+        <v>8.19</v>
       </c>
       <c r="J7">
         <v>1025</v>
       </c>
       <c r="K7">
-        <v>255304</v>
+        <v>6730229</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -10862,31 +10383,31 @@
         <v>25</v>
       </c>
       <c r="B8">
-        <v>5.3448333333333329</v>
+        <v>4.3491666666666662</v>
       </c>
       <c r="C8">
-        <v>10.01</v>
+        <v>8.23</v>
       </c>
       <c r="D8">
         <v>1027</v>
       </c>
       <c r="E8">
-        <v>258847</v>
+        <v>7721557</v>
       </c>
       <c r="G8">
         <v>8</v>
       </c>
       <c r="H8">
-        <v>6.0679999999999996</v>
+        <v>5.0908333333333333</v>
       </c>
       <c r="I8">
-        <v>11.27</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="J8">
         <v>1027</v>
       </c>
       <c r="K8">
-        <v>258627</v>
+        <v>7715900</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -10894,31 +10415,31 @@
         <v>26</v>
       </c>
       <c r="B9">
-        <v>3.0766666666666667</v>
+        <v>4.153833333333333</v>
       </c>
       <c r="C9">
-        <v>5.74</v>
+        <v>8.06</v>
       </c>
       <c r="D9">
         <v>1028</v>
       </c>
       <c r="E9">
-        <v>202110</v>
+        <v>5653496</v>
       </c>
       <c r="G9">
         <v>9</v>
       </c>
       <c r="H9">
-        <v>3.6955</v>
+        <v>4.8711666666666664</v>
       </c>
       <c r="I9">
-        <v>6.8500000000000005</v>
+        <v>9.34</v>
       </c>
       <c r="J9">
         <v>1028</v>
       </c>
       <c r="K9">
-        <v>202058</v>
+        <v>6270341</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -10926,31 +10447,31 @@
         <v>27</v>
       </c>
       <c r="B10">
-        <v>4.1661666666666664</v>
+        <v>4.1875</v>
       </c>
       <c r="C10">
-        <v>7.9600000000000009</v>
+        <v>8.08</v>
       </c>
       <c r="D10">
         <v>1028</v>
       </c>
       <c r="E10">
-        <v>227199</v>
+        <v>7383244</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
       <c r="H10">
-        <v>4.7540000000000004</v>
+        <v>4.782</v>
       </c>
       <c r="I10">
-        <v>9.0399999999999991</v>
+        <v>9.1800000000000015</v>
       </c>
       <c r="J10">
         <v>1028</v>
       </c>
       <c r="K10">
-        <v>227042</v>
+        <v>7378971</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -10958,31 +10479,31 @@
         <v>28</v>
       </c>
       <c r="B11">
-        <v>4.1091666666666669</v>
+        <v>3.3935000000000004</v>
       </c>
       <c r="C11">
-        <v>8.0500000000000007</v>
+        <v>6.7299999999999995</v>
       </c>
       <c r="D11">
         <v>1028</v>
       </c>
       <c r="E11">
-        <v>259623</v>
+        <v>6587300</v>
       </c>
       <c r="G11">
         <v>11</v>
       </c>
       <c r="H11">
-        <v>4.6979999999999995</v>
+        <v>5.1733333333333329</v>
       </c>
       <c r="I11">
-        <v>9.1300000000000008</v>
+        <v>8.73</v>
       </c>
       <c r="J11">
         <v>1028</v>
       </c>
       <c r="K11">
-        <v>259471</v>
+        <v>6845481</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -10990,51 +10511,63 @@
         <v>29</v>
       </c>
       <c r="B12">
-        <v>2.2314999999999996</v>
+        <v>2.9376666666666664</v>
       </c>
       <c r="C12">
-        <v>4.78</v>
+        <v>5.82</v>
       </c>
       <c r="D12">
         <v>1025</v>
       </c>
       <c r="E12">
-        <v>254596</v>
+        <v>7289034</v>
       </c>
       <c r="G12">
         <v>12</v>
       </c>
       <c r="H12">
-        <v>3.1671666666666667</v>
+        <v>3.5665</v>
       </c>
       <c r="I12">
-        <v>6.34</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="J12">
         <v>1025</v>
       </c>
       <c r="K12">
-        <v>254238</v>
+        <v>7283662</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
+      <c r="B13">
+        <v>3.3136666666666668</v>
+      </c>
+      <c r="C13">
+        <v>6.08</v>
+      </c>
+      <c r="D13">
+        <v>1029</v>
+      </c>
+      <c r="E13">
+        <v>6729657</v>
+      </c>
       <c r="G13">
         <v>13</v>
       </c>
       <c r="H13">
-        <v>2.7395</v>
+        <v>3.9063333333333334</v>
       </c>
       <c r="I13">
-        <v>5.7799999999999994</v>
+        <v>7.39</v>
       </c>
       <c r="J13">
         <v>1029</v>
       </c>
       <c r="K13">
-        <v>260544</v>
+        <v>6978768</v>
       </c>
     </row>
   </sheetData>
@@ -55845,8 +55378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56904,8 +56437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V29" sqref="V29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update result and update codes for dedicated APC
</commit_message>
<xml_diff>
--- a/doc/APC-GTFS.xlsx
+++ b/doc/APC-GTFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ro2_apc" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1012,7 +1012,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1116,7 +1115,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2505,7 +2503,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -38638,7 +38635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I271"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A255" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -49788,15 +49785,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I271"/>
+  <dimension ref="A2:M275"/>
   <sheetViews>
-    <sheetView topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="I271" sqref="I271"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="N273" sqref="N273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20180507</v>
       </c>
@@ -49816,8 +49813,12 @@
         <f t="shared" ref="G2:G65" si="0">D2*C2</f>
         <v>71600438</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>E2*C2</f>
+        <v>21963.005999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20180508</v>
       </c>
@@ -49837,8 +49838,12 @@
         <f t="shared" si="0"/>
         <v>71180557.709999993</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f t="shared" ref="I3:I66" si="1">E3*C3</f>
+        <v>22472.360999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20180509</v>
       </c>
@@ -49858,8 +49863,12 @@
         <f t="shared" si="0"/>
         <v>67887145.61999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>20642.588400000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20180510</v>
       </c>
@@ -49879,8 +49888,12 @@
         <f t="shared" si="0"/>
         <v>69047312.399999991</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>21356.698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20180511</v>
       </c>
@@ -49900,8 +49913,12 @@
         <f t="shared" si="0"/>
         <v>65991265.199999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>19867.3125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20180512</v>
       </c>
@@ -49921,8 +49938,12 @@
         <f t="shared" si="0"/>
         <v>50748931.920000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>15573.999200000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20180513</v>
       </c>
@@ -49942,8 +49963,12 @@
         <f t="shared" si="0"/>
         <v>38509406.670000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>11519.361000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20180514</v>
       </c>
@@ -49963,8 +49988,12 @@
         <f t="shared" si="0"/>
         <v>54945862.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>17305.054800000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20180515</v>
       </c>
@@ -49984,8 +50013,12 @@
         <f t="shared" si="0"/>
         <v>74493083.280000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>21537.2703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20180516</v>
       </c>
@@ -50005,8 +50038,12 @@
         <f t="shared" si="0"/>
         <v>66414354.959999993</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>20048.589600000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20180517</v>
       </c>
@@ -50026,8 +50063,12 @@
         <f t="shared" si="0"/>
         <v>71380682.489999995</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>22438.811399999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20180518</v>
       </c>
@@ -50047,8 +50088,12 @@
         <f t="shared" si="0"/>
         <v>73351862.100000009</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>22604.579999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20180519</v>
       </c>
@@ -50068,8 +50113,12 @@
         <f t="shared" si="0"/>
         <v>57426040.439999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>19284.355800000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20180520</v>
       </c>
@@ -50089,8 +50138,12 @@
         <f t="shared" si="0"/>
         <v>50094693.329999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>15221.629499999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20180521</v>
       </c>
@@ -50110,8 +50163,12 @@
         <f t="shared" si="0"/>
         <v>60662424.100000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>20269.129499999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20180522</v>
       </c>
@@ -50131,8 +50188,12 @@
         <f t="shared" si="0"/>
         <v>67834046.280000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>21771.149399999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20180523</v>
       </c>
@@ -50152,8 +50213,12 @@
         <f t="shared" si="0"/>
         <v>73938089.200000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>22919.667999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20180524</v>
       </c>
@@ -50173,8 +50238,12 @@
         <f t="shared" si="0"/>
         <v>68030247.820000008</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>21072.803</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20180525</v>
       </c>
@@ -50194,8 +50263,12 @@
         <f t="shared" si="0"/>
         <v>69838869.320000008</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>21335.914400000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20180526</v>
       </c>
@@ -50215,8 +50288,12 @@
         <f t="shared" si="0"/>
         <v>47572193.699999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>15364.614500000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20180527</v>
       </c>
@@ -50236,8 +50313,12 @@
         <f t="shared" si="0"/>
         <v>42704365.199999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>12875.688</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20180528</v>
       </c>
@@ -50248,8 +50329,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20180529</v>
       </c>
@@ -50269,8 +50354,12 @@
         <f t="shared" si="0"/>
         <v>64574257.399999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>21110.212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20180530</v>
       </c>
@@ -50290,8 +50379,12 @@
         <f t="shared" si="0"/>
         <v>77409016.179999992</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>22664.393200000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20180531</v>
       </c>
@@ -50311,8 +50404,12 @@
         <f t="shared" si="0"/>
         <v>76754493.609999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>23931.315999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20180601</v>
       </c>
@@ -50332,8 +50429,12 @@
         <f t="shared" si="0"/>
         <v>82042874.760000005</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>26222.918399999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20180602</v>
       </c>
@@ -50353,8 +50454,12 @@
         <f t="shared" si="0"/>
         <v>73039945.150000006</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>22844.4329</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20180603</v>
       </c>
@@ -50374,8 +50479,12 @@
         <f t="shared" si="0"/>
         <v>41807982.420000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>12559.4712</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20180604</v>
       </c>
@@ -50395,8 +50504,12 @@
         <f t="shared" si="0"/>
         <v>67362784</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>21440.761599999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20180605</v>
       </c>
@@ -50416,8 +50529,12 @@
         <f t="shared" si="0"/>
         <v>69175749.719999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>22562.9218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>20180606</v>
       </c>
@@ -50437,8 +50554,12 @@
         <f t="shared" si="0"/>
         <v>73677252</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>23350.829600000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20180607</v>
       </c>
@@ -50458,8 +50579,12 @@
         <f t="shared" si="0"/>
         <v>77427877.320000008</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>23421.921000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20180608</v>
       </c>
@@ -50479,8 +50604,12 @@
         <f t="shared" si="0"/>
         <v>82512811.260000005</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>24134.763299999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20180609</v>
       </c>
@@ -50500,8 +50629,12 @@
         <f t="shared" si="0"/>
         <v>61340040.079999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>19985.763600000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>20180610</v>
       </c>
@@ -50521,8 +50654,12 @@
         <f t="shared" si="0"/>
         <v>46043814.960000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>13518.720600000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>20180611</v>
       </c>
@@ -50542,8 +50679,12 @@
         <f t="shared" si="0"/>
         <v>55453642.739999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>17179.656300000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>20180612</v>
       </c>
@@ -50563,8 +50704,12 @@
         <f t="shared" si="0"/>
         <v>73283933.030000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>23392.091800000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20180613</v>
       </c>
@@ -50584,8 +50729,12 @@
         <f t="shared" si="0"/>
         <v>97011351.780000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>28509.055400000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>20180614</v>
       </c>
@@ -50605,8 +50754,12 @@
         <f t="shared" si="0"/>
         <v>102358588.68000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>30470.669099999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20180615</v>
       </c>
@@ -50626,8 +50779,12 @@
         <f t="shared" si="0"/>
         <v>114189420.14999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>32853.190499999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>20180616</v>
       </c>
@@ -50647,8 +50804,12 @@
         <f t="shared" si="0"/>
         <v>76105039.120000005</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>24730.554400000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>20180617</v>
       </c>
@@ -50668,8 +50829,12 @@
         <f t="shared" si="0"/>
         <v>42577092.25</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>12955.827499999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>20180618</v>
       </c>
@@ -50689,8 +50854,12 @@
         <f t="shared" si="0"/>
         <v>59390725.140000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>19626.468000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>20180619</v>
       </c>
@@ -50710,8 +50879,12 @@
         <f t="shared" si="0"/>
         <v>66753404.219999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>21766.848399999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>20180620</v>
       </c>
@@ -50731,8 +50904,12 @@
         <f t="shared" si="0"/>
         <v>70583971.100000009</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>23213.479600000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20180621</v>
       </c>
@@ -50752,8 +50929,12 @@
         <f t="shared" si="0"/>
         <v>105474051.33999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>30197.760200000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20180622</v>
       </c>
@@ -50773,8 +50954,12 @@
         <f t="shared" si="0"/>
         <v>72075164.459999993</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>22182.555199999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>20180623</v>
       </c>
@@ -50794,8 +50979,12 @@
         <f t="shared" si="0"/>
         <v>75784538.659999996</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>23720.754700000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20180624</v>
       </c>
@@ -50815,8 +51004,12 @@
         <f t="shared" si="0"/>
         <v>52878880.979999997</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>16044.8022</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20180625</v>
       </c>
@@ -50836,8 +51029,12 @@
         <f t="shared" si="0"/>
         <v>59251078.560000002</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>20444.843400000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>20180626</v>
       </c>
@@ -50857,8 +51054,12 @@
         <f t="shared" si="0"/>
         <v>88844616.200000003</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>26718.639999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>20180627</v>
       </c>
@@ -50878,8 +51079,12 @@
         <f t="shared" si="0"/>
         <v>64570445.100000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>20642.857899999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>20180628</v>
       </c>
@@ -50899,8 +51104,12 @@
         <f t="shared" si="0"/>
         <v>69724528.280000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>21854.6152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>20180629</v>
       </c>
@@ -50920,8 +51129,12 @@
         <f t="shared" si="0"/>
         <v>84008344.160000011</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>26448.142399999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20180630</v>
       </c>
@@ -50941,8 +51154,12 @@
         <f t="shared" si="0"/>
         <v>54937485.149999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>16960.786</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>20180701</v>
       </c>
@@ -50962,8 +51179,12 @@
         <f t="shared" si="0"/>
         <v>43253342.580000006</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <f t="shared" si="1"/>
+        <v>13001.8833</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>20180702</v>
       </c>
@@ -50983,8 +51204,12 @@
         <f t="shared" si="0"/>
         <v>63574847.119999997</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>20065.5834</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>20180703</v>
       </c>
@@ -50995,8 +51220,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>20180704</v>
       </c>
@@ -51007,8 +51236,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>20180705</v>
       </c>
@@ -51028,8 +51261,12 @@
         <f t="shared" si="0"/>
         <v>58342937.190000005</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>19300.569200000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>20180706</v>
       </c>
@@ -51049,8 +51286,12 @@
         <f t="shared" si="0"/>
         <v>69109538.189999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <f t="shared" si="1"/>
+        <v>21591.108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>20180707</v>
       </c>
@@ -51070,8 +51311,12 @@
         <f t="shared" si="0"/>
         <v>63012456.000000007</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <f t="shared" si="1"/>
+        <v>19427.962499999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>20180708</v>
       </c>
@@ -51091,8 +51336,12 @@
         <f t="shared" si="0"/>
         <v>43411524.530000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <f t="shared" si="1"/>
+        <v>13129.0082</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>20180709</v>
       </c>
@@ -51112,8 +51361,12 @@
         <f t="shared" si="0"/>
         <v>65783187.57</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>21358.680899999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>20180710</v>
       </c>
@@ -51121,11 +51374,15 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <f t="shared" ref="G66:G129" si="1">D66*C66</f>
+        <f t="shared" ref="G66:G129" si="2">D66*C66</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>20180711</v>
       </c>
@@ -51142,11 +51399,15 @@
         <v>8.3699999999999997E-2</v>
       </c>
       <c r="G67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67631546.289999992</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <f t="shared" ref="I67:I130" si="3">E67*C67</f>
+        <v>21506.631300000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>20180712</v>
       </c>
@@ -51163,11 +51424,15 @@
         <v>9.0899999999999995E-2</v>
       </c>
       <c r="G68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71885754.599999994</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <f t="shared" si="3"/>
+        <v>23141.322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>20180713</v>
       </c>
@@ -51184,11 +51449,15 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="G69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68174326.219999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <f t="shared" si="3"/>
+        <v>21798.545999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>20180714</v>
       </c>
@@ -51205,11 +51474,15 @@
         <v>7.6100000000000001E-2</v>
       </c>
       <c r="G70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54522940.079999998</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <f t="shared" si="3"/>
+        <v>16965.962299999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>20180715</v>
       </c>
@@ -51226,11 +51499,15 @@
         <v>6.7599999999999993E-2</v>
       </c>
       <c r="G71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44433011.25</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <f t="shared" si="3"/>
+        <v>13765.05</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>20180716</v>
       </c>
@@ -51247,11 +51524,15 @@
         <v>9.0300000000000005E-2</v>
       </c>
       <c r="G72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>74383078.320000008</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <f t="shared" si="3"/>
+        <v>23158.1574</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>20180717</v>
       </c>
@@ -51268,11 +51549,15 @@
         <v>8.3799999999999999E-2</v>
       </c>
       <c r="G73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66930816.240000002</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <f t="shared" si="3"/>
+        <v>21162.0978</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>20180718</v>
       </c>
@@ -51289,11 +51574,15 @@
         <v>8.5099999999999995E-2</v>
       </c>
       <c r="G74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68472256.430000007</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <f t="shared" si="3"/>
+        <v>21409.372899999998</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>20180719</v>
       </c>
@@ -51310,11 +51599,15 @@
         <v>9.69E-2</v>
       </c>
       <c r="G75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67486029.960000008</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <f t="shared" si="3"/>
+        <v>20877.2988</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20180720</v>
       </c>
@@ -51331,11 +51624,15 @@
         <v>0.1045</v>
       </c>
       <c r="G76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87125532.25999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <f t="shared" si="3"/>
+        <v>26638.826499999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>20180721</v>
       </c>
@@ -51352,11 +51649,15 @@
         <v>7.7700000000000005E-2</v>
       </c>
       <c r="G77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58390050.82</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <f t="shared" si="3"/>
+        <v>17529.197700000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>20180722</v>
       </c>
@@ -51373,11 +51674,15 @@
         <v>7.1900000000000006E-2</v>
       </c>
       <c r="G78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47666940.75</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <f t="shared" si="3"/>
+        <v>14414.152500000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>20180723</v>
       </c>
@@ -51394,11 +51699,15 @@
         <v>7.9899999999999999E-2</v>
       </c>
       <c r="G79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62082578.559999995</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <f t="shared" si="3"/>
+        <v>20419.8832</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>20180724</v>
       </c>
@@ -51415,11 +51724,15 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="G80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65845212.789999999</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <f t="shared" si="3"/>
+        <v>21135.625700000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>20180725</v>
       </c>
@@ -51436,11 +51749,15 @@
         <v>8.2699999999999996E-2</v>
       </c>
       <c r="G81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67763644.620000005</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <f t="shared" si="3"/>
+        <v>21168.140100000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>20180726</v>
       </c>
@@ -51457,11 +51774,15 @@
         <v>8.1100000000000005E-2</v>
       </c>
       <c r="G82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63449581.079999998</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <f t="shared" si="3"/>
+        <v>21038.313200000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>20180727</v>
       </c>
@@ -51478,11 +51799,15 @@
         <v>8.5900000000000004E-2</v>
       </c>
       <c r="G83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67006703.780000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <f t="shared" si="3"/>
+        <v>22160.9974</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>20180728</v>
       </c>
@@ -51499,11 +51824,15 @@
         <v>7.7700000000000005E-2</v>
       </c>
       <c r="G84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56165286.539999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <f t="shared" si="3"/>
+        <v>17810.238600000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>20180729</v>
       </c>
@@ -51520,11 +51849,15 @@
         <v>7.3499999999999996E-2</v>
       </c>
       <c r="G85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48955381.799999997</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <f t="shared" si="3"/>
+        <v>14910.577499999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>20180730</v>
       </c>
@@ -51541,11 +51874,15 @@
         <v>8.3900000000000002E-2</v>
       </c>
       <c r="G86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66932019.780000009</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <f t="shared" si="3"/>
+        <v>21518.168600000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>20180731</v>
       </c>
@@ -51562,11 +51899,15 @@
         <v>8.1500000000000003E-2</v>
       </c>
       <c r="G87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65171452.080000006</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <f t="shared" si="3"/>
+        <v>20807.276000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>20180801</v>
       </c>
@@ -51583,11 +51924,15 @@
         <v>9.0200000000000002E-2</v>
       </c>
       <c r="G88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71843178.599999994</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <f t="shared" si="3"/>
+        <v>23079.474000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>20180802</v>
       </c>
@@ -51604,11 +51949,15 @@
         <v>8.7900000000000006E-2</v>
       </c>
       <c r="G89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69057997.260000005</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <f t="shared" si="3"/>
+        <v>22929.769800000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>20180803</v>
       </c>
@@ -51625,11 +51974,15 @@
         <v>0.1188</v>
       </c>
       <c r="G90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102253030.40000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <f t="shared" si="3"/>
+        <v>30808.166400000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>20180804</v>
       </c>
@@ -51646,11 +51999,15 @@
         <v>9.1700000000000004E-2</v>
       </c>
       <c r="G91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65012889.280000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <f t="shared" si="3"/>
+        <v>20540.5249</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>20180805</v>
       </c>
@@ -51667,11 +52024,15 @@
         <v>7.6600000000000001E-2</v>
       </c>
       <c r="G92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52485005.280000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I92">
+        <f t="shared" si="3"/>
+        <v>15466.459200000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>20180806</v>
       </c>
@@ -51688,11 +52049,15 @@
         <v>8.1199999999999994E-2</v>
       </c>
       <c r="G93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65438289.440000005</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <f t="shared" si="3"/>
+        <v>21141.881599999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>20180807</v>
       </c>
@@ -51709,11 +52074,15 @@
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72209922.850000009</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I94">
+        <f t="shared" si="3"/>
+        <v>22521.362499999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>20180808</v>
       </c>
@@ -51730,11 +52099,15 @@
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="G95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>61522941.959999993</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I95">
+        <f t="shared" si="3"/>
+        <v>20085.21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>20180809</v>
       </c>
@@ -51751,11 +52124,15 @@
         <v>8.2900000000000001E-2</v>
       </c>
       <c r="G96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66387225.019999996</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I96">
+        <f t="shared" si="3"/>
+        <v>21515.700199999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>20180810</v>
       </c>
@@ -51772,11 +52149,15 @@
         <v>9.0300000000000005E-2</v>
       </c>
       <c r="G97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71531047.539999992</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <f t="shared" si="3"/>
+        <v>23610.108900000003</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>20180811</v>
       </c>
@@ -51793,11 +52174,15 @@
         <v>7.4099999999999999E-2</v>
       </c>
       <c r="G98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54618922.549999997</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I98">
+        <f t="shared" si="3"/>
+        <v>17279.0085</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>20180812</v>
       </c>
@@ -51814,11 +52199,15 @@
         <v>7.1300000000000002E-2</v>
       </c>
       <c r="G99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>49412974.240000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I99">
+        <f t="shared" si="3"/>
+        <v>14861.2016</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>20180813</v>
       </c>
@@ -51835,11 +52224,15 @@
         <v>8.3599999999999994E-2</v>
       </c>
       <c r="G100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65233091.990000002</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I100">
+        <f t="shared" si="3"/>
+        <v>21849.779599999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>20180814</v>
       </c>
@@ -51856,11 +52249,15 @@
         <v>8.6800000000000002E-2</v>
       </c>
       <c r="G101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66994890</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I101">
+        <f t="shared" si="3"/>
+        <v>21877.940000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>20180815</v>
       </c>
@@ -51877,11 +52274,15 @@
         <v>8.8499999999999995E-2</v>
       </c>
       <c r="G102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>69392436.75</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I102">
+        <f t="shared" si="3"/>
+        <v>23328.511500000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>20180816</v>
       </c>
@@ -51898,11 +52299,15 @@
         <v>0.1067</v>
       </c>
       <c r="G103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>87562094.700000003</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I103">
+        <f t="shared" si="3"/>
+        <v>27781.372299999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>20180817</v>
       </c>
@@ -51919,11 +52324,15 @@
         <v>9.7600000000000006E-2</v>
       </c>
       <c r="G104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82508440.950000003</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I104">
+        <f t="shared" si="3"/>
+        <v>25439.342400000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>20180818</v>
       </c>
@@ -51940,11 +52349,15 @@
         <v>9.6600000000000005E-2</v>
       </c>
       <c r="G105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71734315.540000007</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I105">
+        <f t="shared" si="3"/>
+        <v>22468.580400000003</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>20180819</v>
       </c>
@@ -51961,11 +52374,15 @@
         <v>7.9200000000000007E-2</v>
       </c>
       <c r="G106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>54530651.269999996</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I106">
+        <f t="shared" si="3"/>
+        <v>16174.778400000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>20180820</v>
       </c>
@@ -51982,11 +52399,15 @@
         <v>0.1081</v>
       </c>
       <c r="G107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91744730.88000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I107">
+        <f t="shared" si="3"/>
+        <v>28387.924800000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>20180821</v>
       </c>
@@ -52003,11 +52424,15 @@
         <v>0.1227</v>
       </c>
       <c r="G108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110942902.11</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I108">
+        <f t="shared" si="3"/>
+        <v>31977.951300000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>20180822</v>
       </c>
@@ -52024,11 +52449,15 @@
         <v>0.1056</v>
       </c>
       <c r="G109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92813462.820000008</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <f t="shared" si="3"/>
+        <v>27795.081600000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>20180823</v>
       </c>
@@ -52045,11 +52474,15 @@
         <v>0.1094</v>
       </c>
       <c r="G110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91771792.489999995</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I110">
+        <f t="shared" si="3"/>
+        <v>28313.9234</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>20180824</v>
       </c>
@@ -52066,11 +52499,15 @@
         <v>0.1321</v>
       </c>
       <c r="G111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111747390.3</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I111">
+        <f t="shared" si="3"/>
+        <v>33923.544199999997</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>20180825</v>
       </c>
@@ -52087,11 +52524,15 @@
         <v>8.2900000000000001E-2</v>
       </c>
       <c r="G112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60133804.339999996</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I112">
+        <f t="shared" si="3"/>
+        <v>19121.2166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>20180826</v>
       </c>
@@ -52108,11 +52549,15 @@
         <v>8.4199999999999997E-2</v>
       </c>
       <c r="G113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>55703567.199999996</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I113">
+        <f t="shared" si="3"/>
+        <v>17046.121599999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>20180827</v>
       </c>
@@ -52129,11 +52574,15 @@
         <v>0.10150000000000001</v>
       </c>
       <c r="G114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83415356.310000002</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I114">
+        <f t="shared" si="3"/>
+        <v>26082.556500000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>20180828</v>
       </c>
@@ -52150,11 +52599,15 @@
         <v>0.108</v>
       </c>
       <c r="G115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91841771.450000003</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I115">
+        <f t="shared" si="3"/>
+        <v>28555.955999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>20180829</v>
       </c>
@@ -52171,11 +52624,15 @@
         <v>9.7900000000000001E-2</v>
       </c>
       <c r="G116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84314068.159999996</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I116">
+        <f t="shared" si="3"/>
+        <v>25775.5036</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>20180830</v>
       </c>
@@ -52192,11 +52649,15 @@
         <v>0.10580000000000001</v>
       </c>
       <c r="G117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>88493028.760000005</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I117">
+        <f t="shared" si="3"/>
+        <v>27624.697400000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>20180831</v>
       </c>
@@ -52213,11 +52674,15 @@
         <v>0.11269999999999999</v>
       </c>
       <c r="G118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94160918.159999996</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I118">
+        <f t="shared" si="3"/>
+        <v>29147.262899999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>20180901</v>
       </c>
@@ -52234,11 +52699,15 @@
         <v>0.1056</v>
       </c>
       <c r="G119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77328597.24000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I119">
+        <f t="shared" si="3"/>
+        <v>24469.315200000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>20180902</v>
       </c>
@@ -52246,11 +52715,15 @@
         <v>0</v>
       </c>
       <c r="G120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I120">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>20180903</v>
       </c>
@@ -52258,11 +52731,15 @@
         <v>0</v>
       </c>
       <c r="G121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I121">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>20180904</v>
       </c>
@@ -52279,11 +52756,15 @@
         <v>0.1011</v>
       </c>
       <c r="G122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80470219.61999999</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I122">
+        <f t="shared" si="3"/>
+        <v>26644.1973</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>20180905</v>
       </c>
@@ -52300,11 +52781,15 @@
         <v>9.1600000000000001E-2</v>
       </c>
       <c r="G123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>72120196.49000001</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I123">
+        <f t="shared" si="3"/>
+        <v>24046.1908</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>20180906</v>
       </c>
@@ -52321,11 +52806,15 @@
         <v>9.9099999999999994E-2</v>
       </c>
       <c r="G124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80624318.390000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I124">
+        <f t="shared" si="3"/>
+        <v>25967.272099999998</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>20180907</v>
       </c>
@@ -52342,11 +52831,15 @@
         <v>0.1021</v>
       </c>
       <c r="G125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>84855752.440000013</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I125">
+        <f t="shared" si="3"/>
+        <v>26763.166699999998</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>20180908</v>
       </c>
@@ -52363,11 +52856,15 @@
         <v>8.9300000000000004E-2</v>
       </c>
       <c r="G126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>63419802</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I126">
+        <f t="shared" si="3"/>
+        <v>20575.434400000002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>20180909</v>
       </c>
@@ -52384,11 +52881,15 @@
         <v>7.6399999999999996E-2</v>
       </c>
       <c r="G127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46975095.75</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I127">
+        <f t="shared" si="3"/>
+        <v>15224.609999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>20180910</v>
       </c>
@@ -52405,11 +52906,15 @@
         <v>8.8599999999999998E-2</v>
       </c>
       <c r="G128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67497237.820000008</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I128">
+        <f t="shared" si="3"/>
+        <v>22326.048200000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>20180911</v>
       </c>
@@ -52426,11 +52931,15 @@
         <v>9.7600000000000006E-2</v>
       </c>
       <c r="G129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>78047637.739999995</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I129">
+        <f t="shared" si="3"/>
+        <v>24882.241600000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>20180912</v>
       </c>
@@ -52447,11 +52956,15 @@
         <v>7.3200000000000001E-2</v>
       </c>
       <c r="G130">
-        <f t="shared" ref="G130:G193" si="2">D130*C130</f>
+        <f t="shared" ref="G130:G193" si="4">D130*C130</f>
         <v>11953425.270000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I130">
+        <f t="shared" si="3"/>
+        <v>4030.1723999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>20180913</v>
       </c>
@@ -52459,11 +52972,15 @@
         <v>0</v>
       </c>
       <c r="G131">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I131">
+        <f t="shared" ref="I131:I194" si="5">E131*C131</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>20180914</v>
       </c>
@@ -52480,11 +52997,15 @@
         <v>0.13950000000000001</v>
       </c>
       <c r="G132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56907475.359999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I132">
+        <f t="shared" si="5"/>
+        <v>17357.427000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>20180915</v>
       </c>
@@ -52501,11 +53022,15 @@
         <v>9.2100000000000001E-2</v>
       </c>
       <c r="G133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65068596.539999992</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I133">
+        <f t="shared" si="5"/>
+        <v>21300.980100000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>20180916</v>
       </c>
@@ -52522,11 +53047,15 @@
         <v>8.1600000000000006E-2</v>
       </c>
       <c r="G134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>52175831.25</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I134">
+        <f t="shared" si="5"/>
+        <v>16945.464</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>20180917</v>
       </c>
@@ -52543,11 +53072,15 @@
         <v>8.6300000000000002E-2</v>
       </c>
       <c r="G135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>68625872</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I135">
+        <f t="shared" si="5"/>
+        <v>22299.920000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>20180918</v>
       </c>
@@ -52564,11 +53097,15 @@
         <v>9.7299999999999998E-2</v>
       </c>
       <c r="G136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>79360026.790000007</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I136">
+        <f t="shared" si="5"/>
+        <v>25332.930700000001</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>20180919</v>
       </c>
@@ -52585,11 +53122,15 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="G137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78444233.099999994</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I137">
+        <f t="shared" si="5"/>
+        <v>24422.73</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>20180920</v>
       </c>
@@ -52606,11 +53147,15 @@
         <v>0.105</v>
       </c>
       <c r="G138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>87653024.150000006</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I138">
+        <f t="shared" si="5"/>
+        <v>27539.924999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>20180921</v>
       </c>
@@ -52627,11 +53172,15 @@
         <v>0.10630000000000001</v>
       </c>
       <c r="G139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>86632485.940000013</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I139">
+        <f t="shared" si="5"/>
+        <v>27574.4326</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>20180922</v>
       </c>
@@ -52648,11 +53197,15 @@
         <v>0.10440000000000001</v>
       </c>
       <c r="G140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>73069294.859999999</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I140">
+        <f t="shared" si="5"/>
+        <v>23686.376400000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>20180923</v>
       </c>
@@ -52669,11 +53222,15 @@
         <v>6.8900000000000003E-2</v>
       </c>
       <c r="G141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40797847.119999997</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I141">
+        <f t="shared" si="5"/>
+        <v>12148.723600000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>20180924</v>
       </c>
@@ -52690,11 +53247,15 @@
         <v>9.6799999999999997E-2</v>
       </c>
       <c r="G142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>78292568.200000003</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I142">
+        <f t="shared" si="5"/>
+        <v>25090.947199999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>20180925</v>
       </c>
@@ -52711,11 +53272,15 @@
         <v>8.5099999999999995E-2</v>
       </c>
       <c r="G143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>67309640.420000002</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I143">
+        <f t="shared" si="5"/>
+        <v>22121.149299999997</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>20180926</v>
       </c>
@@ -52732,11 +53297,15 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="G144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>69783038</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I144">
+        <f t="shared" si="5"/>
+        <v>22481.280000000002</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>20180927</v>
       </c>
@@ -52753,11 +53322,15 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="G145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>82029953.060000002</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I145">
+        <f t="shared" si="5"/>
+        <v>24492.71</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>20180928</v>
       </c>
@@ -52774,11 +53347,15 @@
         <v>0.10059999999999999</v>
       </c>
       <c r="G146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>84050987.099999994</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I146">
+        <f t="shared" si="5"/>
+        <v>26267.565399999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>20180929</v>
       </c>
@@ -52795,11 +53372,15 @@
         <v>7.7600000000000002E-2</v>
       </c>
       <c r="G147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54362982.439999998</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I147">
+        <f t="shared" si="5"/>
+        <v>17597.895199999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>20180930</v>
       </c>
@@ -52816,11 +53397,15 @@
         <v>6.8500000000000005E-2</v>
       </c>
       <c r="G148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44802320.339999996</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I148">
+        <f t="shared" si="5"/>
+        <v>13840.973000000002</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>20181001</v>
       </c>
@@ -52837,11 +53422,15 @@
         <v>9.7299999999999998E-2</v>
       </c>
       <c r="G149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>67498010.400000006</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I149">
+        <f t="shared" si="5"/>
+        <v>22202.6924</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>20181002</v>
       </c>
@@ -52858,11 +53447,15 @@
         <v>9.5899999999999999E-2</v>
       </c>
       <c r="G150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54665556</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I150">
+        <f t="shared" si="5"/>
+        <v>18472.258000000002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>20181003</v>
       </c>
@@ -52879,11 +53472,15 @@
         <v>0.1132</v>
       </c>
       <c r="G151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>79713647.189999998</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I151">
+        <f t="shared" si="5"/>
+        <v>25240.090799999998</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>20181004</v>
       </c>
@@ -52900,11 +53497,15 @@
         <v>0.1046</v>
       </c>
       <c r="G152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>86084346.480000004</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I152">
+        <f t="shared" si="5"/>
+        <v>27059.810799999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>20181005</v>
       </c>
@@ -52921,11 +53522,15 @@
         <v>0.1079</v>
       </c>
       <c r="G153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>69570204.340000004</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I153">
+        <f t="shared" si="5"/>
+        <v>21370.5661</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>20181006</v>
       </c>
@@ -52942,11 +53547,15 @@
         <v>0.1145</v>
       </c>
       <c r="G154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>86870016.280000001</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I154">
+        <f t="shared" si="5"/>
+        <v>26306.146000000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>20181007</v>
       </c>
@@ -52963,11 +53572,15 @@
         <v>8.6699999999999999E-2</v>
       </c>
       <c r="G155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56725175.949999996</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I155">
+        <f t="shared" si="5"/>
+        <v>17757.9807</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>20181008</v>
       </c>
@@ -52984,11 +53597,15 @@
         <v>7.85E-2</v>
       </c>
       <c r="G156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>59641461.119999997</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I156">
+        <f t="shared" si="5"/>
+        <v>20090.348000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>20181009</v>
       </c>
@@ -53005,11 +53622,15 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="G157">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>83266406.640000001</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I157">
+        <f t="shared" si="5"/>
+        <v>25615.656000000003</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>20181010</v>
       </c>
@@ -53026,11 +53647,15 @@
         <v>0.1041</v>
       </c>
       <c r="G158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>88368262.5</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I158">
+        <f t="shared" si="5"/>
+        <v>27016.552499999998</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>20181011</v>
       </c>
@@ -53047,11 +53672,15 @@
         <v>8.8499999999999995E-2</v>
       </c>
       <c r="G159">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>69482445.75999999</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I159">
+        <f t="shared" si="5"/>
+        <v>22512.984</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>20181012</v>
       </c>
@@ -53068,11 +53697,15 @@
         <v>9.8900000000000002E-2</v>
       </c>
       <c r="G160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>83778476.560000002</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I160">
+        <f t="shared" si="5"/>
+        <v>25558.133600000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>20181013</v>
       </c>
@@ -53089,11 +53722,15 @@
         <v>8.8300000000000003E-2</v>
       </c>
       <c r="G161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>62189160.120000005</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I161">
+        <f t="shared" si="5"/>
+        <v>20185.644899999999</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>20181014</v>
       </c>
@@ -53110,11 +53747,15 @@
         <v>6.8900000000000003E-2</v>
       </c>
       <c r="G162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44601942.239999995</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I162">
+        <f t="shared" si="5"/>
+        <v>14005.4408</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>20181015</v>
       </c>
@@ -53131,11 +53772,15 @@
         <v>8.9899999999999994E-2</v>
       </c>
       <c r="G163">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>69739821.659999996</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I163">
+        <f t="shared" si="5"/>
+        <v>23204.4486</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>20181016</v>
       </c>
@@ -53152,11 +53797,15 @@
         <v>8.3900000000000002E-2</v>
       </c>
       <c r="G164">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>67668255.840000004</v>
       </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I164">
+        <f t="shared" si="5"/>
+        <v>21446.685799999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>20181017</v>
       </c>
@@ -53173,11 +53822,15 @@
         <v>8.6400000000000005E-2</v>
       </c>
       <c r="G165">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>66276240.479999997</v>
       </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I165">
+        <f t="shared" si="5"/>
+        <v>22210.329600000001</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>20181018</v>
       </c>
@@ -53194,11 +53847,15 @@
         <v>9.7500000000000003E-2</v>
       </c>
       <c r="G166">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>83240872.299999997</v>
       </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I166">
+        <f t="shared" si="5"/>
+        <v>25077.975000000002</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>20181019</v>
       </c>
@@ -53215,11 +53872,15 @@
         <v>9.8400000000000001E-2</v>
       </c>
       <c r="G167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>81308681.88000001</v>
       </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I167">
+        <f t="shared" si="5"/>
+        <v>24911.337599999999</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>20181020</v>
       </c>
@@ -53236,11 +53897,15 @@
         <v>8.5900000000000004E-2</v>
       </c>
       <c r="G168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>56165965.289999999</v>
       </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I168">
+        <f t="shared" si="5"/>
+        <v>18490.2327</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>20181021</v>
       </c>
@@ -53257,11 +53922,15 @@
         <v>9.3200000000000005E-2</v>
       </c>
       <c r="G169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>51638648.399999999</v>
       </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I169">
+        <f t="shared" si="5"/>
+        <v>17409.0144</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>20181022</v>
       </c>
@@ -53278,11 +53947,15 @@
         <v>8.0299999999999996E-2</v>
       </c>
       <c r="G170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>60434007.230000004</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I170">
+        <f t="shared" si="5"/>
+        <v>20244.673899999998</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>20181023</v>
       </c>
@@ -53299,11 +53972,15 @@
         <v>8.9899999999999994E-2</v>
       </c>
       <c r="G171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>66686197.760000005</v>
       </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I171">
+        <f t="shared" si="5"/>
+        <v>22517.612599999997</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>20181024</v>
       </c>
@@ -53320,11 +53997,15 @@
         <v>8.4599999999999995E-2</v>
       </c>
       <c r="G172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65094472.710000001</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I172">
+        <f t="shared" si="5"/>
+        <v>21902.6862</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>20181025</v>
       </c>
@@ -53341,11 +54022,15 @@
         <v>8.8599999999999998E-2</v>
       </c>
       <c r="G173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>68785763.510000005</v>
       </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I173">
+        <f t="shared" si="5"/>
+        <v>22536.030200000001</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>20181026</v>
       </c>
@@ -53362,11 +54047,15 @@
         <v>0.12039999999999999</v>
       </c>
       <c r="G174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>104867719.74000001</v>
       </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I174">
+        <f t="shared" si="5"/>
+        <v>30811.082399999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>20181027</v>
       </c>
@@ -53383,11 +54072,15 @@
         <v>7.17E-2</v>
       </c>
       <c r="G175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47517263.280000001</v>
       </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I175">
+        <f t="shared" si="5"/>
+        <v>16149.9231</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>20181028</v>
       </c>
@@ -53404,11 +54097,15 @@
         <v>6.6400000000000001E-2</v>
       </c>
       <c r="G176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44026163.100000001</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I176">
+        <f t="shared" si="5"/>
+        <v>13812.1296</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>20181029</v>
       </c>
@@ -53425,11 +54122,15 @@
         <v>8.1900000000000001E-2</v>
       </c>
       <c r="G177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>58801227.100000001</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I177">
+        <f t="shared" si="5"/>
+        <v>20709.643500000002</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>20181030</v>
       </c>
@@ -53446,11 +54147,15 @@
         <v>8.5599999999999996E-2</v>
       </c>
       <c r="G178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>67718043.11999999</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I178">
+        <f t="shared" si="5"/>
+        <v>21987.0448</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>20181031</v>
       </c>
@@ -53467,11 +54172,15 @@
         <v>9.0399999999999994E-2</v>
       </c>
       <c r="G179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>64761460.080000006</v>
       </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I179">
+        <f t="shared" si="5"/>
+        <v>20524.596799999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>20181101</v>
       </c>
@@ -53488,11 +54197,15 @@
         <v>9.9099999999999994E-2</v>
       </c>
       <c r="G180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32487802.739999998</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I180">
+        <f t="shared" si="5"/>
+        <v>10583.285399999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>20181102</v>
       </c>
@@ -53509,11 +54222,15 @@
         <v>9.7699999999999995E-2</v>
       </c>
       <c r="G181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>76306844.140000001</v>
       </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I181">
+        <f t="shared" si="5"/>
+        <v>23738.0713</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>20181103</v>
       </c>
@@ -53530,11 +54247,15 @@
         <v>0.10009999999999999</v>
       </c>
       <c r="G182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>71501745</v>
       </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I182">
+        <f t="shared" si="5"/>
+        <v>23275.852599999998</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>20181104</v>
       </c>
@@ -53551,11 +54272,15 @@
         <v>0.36409999999999998</v>
       </c>
       <c r="G183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>535031457.83999997</v>
       </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I183">
+        <f t="shared" si="5"/>
+        <v>73848.218399999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>20181105</v>
       </c>
@@ -53572,11 +54297,15 @@
         <v>8.3299999999999999E-2</v>
       </c>
       <c r="G184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>64600973.25</v>
       </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I184">
+        <f t="shared" si="5"/>
+        <v>21460.6623</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>20181106</v>
       </c>
@@ -53593,11 +54322,15 @@
         <v>8.4400000000000003E-2</v>
       </c>
       <c r="G185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65676238.800000004</v>
       </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I185">
+        <f t="shared" si="5"/>
+        <v>22048.824800000002</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>20181107</v>
       </c>
@@ -53614,11 +54347,15 @@
         <v>8.5900000000000004E-2</v>
       </c>
       <c r="G186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70182983.519999996</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I186">
+        <f t="shared" si="5"/>
+        <v>22210.1322</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>20181108</v>
       </c>
@@ -53635,11 +54372,15 @@
         <v>7.9500000000000001E-2</v>
       </c>
       <c r="G187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>62202631.899999999</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I187">
+        <f t="shared" si="5"/>
+        <v>20699.494500000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>20181109</v>
       </c>
@@ -53656,11 +54397,15 @@
         <v>8.5400000000000004E-2</v>
       </c>
       <c r="G188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>66017302.560000002</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I188">
+        <f t="shared" si="5"/>
+        <v>22420.574400000001</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>20181110</v>
       </c>
@@ -53677,11 +54422,15 @@
         <v>6.4500000000000002E-2</v>
       </c>
       <c r="G189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45155706.530000001</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I189">
+        <f t="shared" si="5"/>
+        <v>14857.639500000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>20181111</v>
       </c>
@@ -53698,11 +54447,15 @@
         <v>0.06</v>
       </c>
       <c r="G190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39984667.200000003</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I190">
+        <f t="shared" si="5"/>
+        <v>12182.4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>20181112</v>
       </c>
@@ -53719,11 +54472,15 @@
         <v>6.2799999999999995E-2</v>
       </c>
       <c r="G191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44546119.660000004</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I191">
+        <f t="shared" si="5"/>
+        <v>16508.298799999997</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>20181113</v>
       </c>
@@ -53740,11 +54497,15 @@
         <v>8.1100000000000005E-2</v>
       </c>
       <c r="G192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>65090117.579999998</v>
       </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I192">
+        <f t="shared" si="5"/>
+        <v>21175.372200000002</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>20181114</v>
       </c>
@@ -53761,11 +54522,15 @@
         <v>7.5399999999999995E-2</v>
       </c>
       <c r="G193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>57259021.75</v>
       </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I193">
+        <f t="shared" si="5"/>
+        <v>19763.470999999998</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>20181115</v>
       </c>
@@ -53782,11 +54547,15 @@
         <v>9.7299999999999998E-2</v>
       </c>
       <c r="G194">
-        <f t="shared" ref="G194:G257" si="3">D194*C194</f>
+        <f t="shared" ref="G194:G257" si="6">D194*C194</f>
         <v>79735337.849999994</v>
       </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I194">
+        <f t="shared" si="5"/>
+        <v>25193.207899999998</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>20181116</v>
       </c>
@@ -53803,11 +54572,15 @@
         <v>7.8600000000000003E-2</v>
       </c>
       <c r="G195">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>61548207.240000002</v>
       </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I195">
+        <f t="shared" ref="I195:I258" si="7">E195*C195</f>
+        <v>20372.648400000002</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>20181117</v>
       </c>
@@ -53824,11 +54597,15 @@
         <v>6.7500000000000004E-2</v>
       </c>
       <c r="G196">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>46397806.560000002</v>
       </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I196">
+        <f t="shared" si="7"/>
+        <v>15249.060000000001</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>20181118</v>
       </c>
@@ -53845,11 +54622,15 @@
         <v>7.1199999999999999E-2</v>
       </c>
       <c r="G197">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>22465614.080000002</v>
       </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I197">
+        <f t="shared" si="7"/>
+        <v>6916.0832</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>20181119</v>
       </c>
@@ -53866,11 +54647,15 @@
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G198">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>56293317.020000003</v>
       </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I198">
+        <f t="shared" si="7"/>
+        <v>18113.724999999999</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>20181120</v>
       </c>
@@ -53887,11 +54672,15 @@
         <v>7.8600000000000003E-2</v>
       </c>
       <c r="G199">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>61174598.100000001</v>
       </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I199">
+        <f t="shared" si="7"/>
+        <v>19933.352999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>20181121</v>
       </c>
@@ -53908,11 +54697,15 @@
         <v>6.5299999999999997E-2</v>
       </c>
       <c r="G200">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>47012765.280000001</v>
       </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I200">
+        <f t="shared" si="7"/>
+        <v>17047.609799999998</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>20181122</v>
       </c>
@@ -53920,11 +54713,15 @@
         <v>0</v>
       </c>
       <c r="G201">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I201">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>20181123</v>
       </c>
@@ -53941,11 +54738,15 @@
         <v>6.7900000000000002E-2</v>
       </c>
       <c r="G202">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>46826554.240000002</v>
       </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I202">
+        <f t="shared" si="7"/>
+        <v>17874.539199999999</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>20181124</v>
       </c>
@@ -53962,11 +54763,15 @@
         <v>0.09</v>
       </c>
       <c r="G203">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>60192128.780000001</v>
       </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I203">
+        <f t="shared" si="7"/>
+        <v>20190.419999999998</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>20181125</v>
       </c>
@@ -53983,11 +54788,15 @@
         <v>5.5300000000000002E-2</v>
       </c>
       <c r="G204">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>37739373.75</v>
       </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I204">
+        <f t="shared" si="7"/>
+        <v>11175.300500000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>20181126</v>
       </c>
@@ -54004,11 +54813,15 @@
         <v>7.6600000000000001E-2</v>
       </c>
       <c r="G205">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>59015598.25</v>
       </c>
-    </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I205">
+        <f t="shared" si="7"/>
+        <v>19719.061399999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>20181127</v>
       </c>
@@ -54025,11 +54838,15 @@
         <v>8.7400000000000005E-2</v>
       </c>
       <c r="G206">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>71422493.399999991</v>
       </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I206">
+        <f t="shared" si="7"/>
+        <v>22393.191000000003</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>20181128</v>
       </c>
@@ -54046,11 +54863,15 @@
         <v>6.6100000000000006E-2</v>
       </c>
       <c r="G207">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>50966314.560000002</v>
       </c>
-    </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I207">
+        <f t="shared" si="7"/>
+        <v>16993.913400000001</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>20181129</v>
       </c>
@@ -54067,11 +54888,15 @@
         <v>6.8599999999999994E-2</v>
       </c>
       <c r="G208">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>54872043.43</v>
       </c>
-    </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I208">
+        <f t="shared" si="7"/>
+        <v>17686.5206</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>20181130</v>
       </c>
@@ -54088,11 +54913,15 @@
         <v>9.1300000000000006E-2</v>
       </c>
       <c r="G209">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>73139685.480000004</v>
       </c>
-    </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I209">
+        <f t="shared" si="7"/>
+        <v>23689.702300000001</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>20181201</v>
       </c>
@@ -54109,11 +54938,15 @@
         <v>6.9500000000000006E-2</v>
       </c>
       <c r="G210">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>50580769.480000004</v>
       </c>
-    </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I210">
+        <f t="shared" si="7"/>
+        <v>15893.677000000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>20181202</v>
       </c>
@@ -54130,11 +54963,15 @@
         <v>6.9800000000000001E-2</v>
       </c>
       <c r="G211">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>47209389.620000005</v>
       </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I211">
+        <f t="shared" si="7"/>
+        <v>14131.638199999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>20181203</v>
       </c>
@@ -54151,11 +54988,15 @@
         <v>7.7600000000000002E-2</v>
       </c>
       <c r="G212">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>60726720.32</v>
       </c>
-    </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I212">
+        <f t="shared" si="7"/>
+        <v>20235.286400000001</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>20181204</v>
       </c>
@@ -54172,11 +55013,15 @@
         <v>7.7600000000000002E-2</v>
       </c>
       <c r="G213">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>59603556.32</v>
       </c>
-    </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I213">
+        <f t="shared" si="7"/>
+        <v>19759.2104</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>20181205</v>
       </c>
@@ -54193,11 +55038,15 @@
         <v>7.1400000000000005E-2</v>
       </c>
       <c r="G214">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>54342339.18</v>
       </c>
-    </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I214">
+        <f t="shared" si="7"/>
+        <v>18481.675800000001</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>20181206</v>
       </c>
@@ -54214,11 +55063,15 @@
         <v>7.8399999999999997E-2</v>
       </c>
       <c r="G215">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>66774662.780000001</v>
       </c>
-    </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I215">
+        <f t="shared" si="7"/>
+        <v>20273.142400000001</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>20181207</v>
       </c>
@@ -54235,11 +55088,15 @@
         <v>8.2299999999999998E-2</v>
       </c>
       <c r="G216">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>65472482.849999994</v>
       </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I216">
+        <f t="shared" si="7"/>
+        <v>21386.724900000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>20181208</v>
       </c>
@@ -54256,11 +55113,15 @@
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="G217">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>44978574</v>
       </c>
-    </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I217">
+        <f t="shared" si="7"/>
+        <v>14500.555199999999</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>20181209</v>
       </c>
@@ -54277,11 +55138,15 @@
         <v>5.7200000000000001E-2</v>
       </c>
       <c r="G218">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>38013102.399999999</v>
       </c>
-    </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I218">
+        <f t="shared" si="7"/>
+        <v>11487.476000000001</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>20181210</v>
       </c>
@@ -54298,11 +55163,15 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="G219">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>49317442.719999999</v>
       </c>
-    </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I219">
+        <f t="shared" si="7"/>
+        <v>18031.494000000002</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>20181211</v>
       </c>
@@ -54319,11 +55188,15 @@
         <v>7.5399999999999995E-2</v>
       </c>
       <c r="G220">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>61353524.880000003</v>
       </c>
-    </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I220">
+        <f t="shared" si="7"/>
+        <v>19489.618199999997</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>20181212</v>
       </c>
@@ -54340,11 +55213,15 @@
         <v>6.93E-2</v>
       </c>
       <c r="G221">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>55103703.299999997</v>
       </c>
-    </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I221">
+        <f t="shared" si="7"/>
+        <v>17745.651000000002</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>20181213</v>
       </c>
@@ -54361,11 +55238,15 @@
         <v>7.2700000000000001E-2</v>
       </c>
       <c r="G222">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>58084749.959999993</v>
       </c>
-    </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I222">
+        <f t="shared" si="7"/>
+        <v>18712.107599999999</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>20181214</v>
       </c>
@@ -54382,11 +55263,15 @@
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G223">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>67427961.959999993</v>
       </c>
-    </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I223">
+        <f t="shared" si="7"/>
+        <v>22325.449999999997</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>20181215</v>
       </c>
@@ -54403,11 +55288,15 @@
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="G224">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45909873.899999999</v>
       </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I224">
+        <f t="shared" si="7"/>
+        <v>14593.867199999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>20181216</v>
       </c>
@@ -54424,11 +55313,15 @@
         <v>5.9900000000000002E-2</v>
       </c>
       <c r="G225">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>40342927.060000002</v>
       </c>
-    </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I225">
+        <f t="shared" si="7"/>
+        <v>12151.972900000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>20181217</v>
       </c>
@@ -54445,11 +55338,15 @@
         <v>7.1199999999999999E-2</v>
       </c>
       <c r="G226">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>54766024.099999994</v>
       </c>
-    </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I226">
+        <f t="shared" si="7"/>
+        <v>18489.928</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>20181218</v>
       </c>
@@ -54466,11 +55363,15 @@
         <v>7.3499999999999996E-2</v>
       </c>
       <c r="G227">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>55239008.939999998</v>
       </c>
-    </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I227">
+        <f t="shared" si="7"/>
+        <v>18877.886999999999</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>20181219</v>
       </c>
@@ -54487,11 +55388,15 @@
         <v>8.4699999999999998E-2</v>
       </c>
       <c r="G228">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>67770797.899999991</v>
       </c>
-    </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I228">
+        <f t="shared" si="7"/>
+        <v>21924.1715</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>20181220</v>
       </c>
@@ -54508,11 +55413,15 @@
         <v>8.1500000000000003E-2</v>
       </c>
       <c r="G229">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>66142549.440000005</v>
       </c>
-    </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I229">
+        <f t="shared" si="7"/>
+        <v>20945.826000000001</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>20181221</v>
       </c>
@@ -54529,11 +55438,15 @@
         <v>8.3599999999999994E-2</v>
       </c>
       <c r="G230">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>66083030.240000002</v>
       </c>
-    </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I230">
+        <f t="shared" si="7"/>
+        <v>21791.343199999999</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>20181222</v>
       </c>
@@ -54550,11 +55463,15 @@
         <v>6.2899999999999998E-2</v>
       </c>
       <c r="G231">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>42526232.310000002</v>
       </c>
-    </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I231">
+        <f t="shared" si="7"/>
+        <v>14203.2603</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>20181223</v>
       </c>
@@ -54571,11 +55488,15 @@
         <v>5.4600000000000003E-2</v>
       </c>
       <c r="G232">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>37648470.460000001</v>
       </c>
-    </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I232">
+        <f t="shared" si="7"/>
+        <v>11143.9146</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>20181224</v>
       </c>
@@ -54592,11 +55513,15 @@
         <v>6.2E-2</v>
       </c>
       <c r="G233">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>46027162.689999998</v>
       </c>
-    </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I233">
+        <f t="shared" si="7"/>
+        <v>16101.585999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>20181225</v>
       </c>
@@ -54604,11 +55529,15 @@
         <v>0</v>
       </c>
       <c r="G234">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I234">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>20181226</v>
       </c>
@@ -54625,11 +55554,15 @@
         <v>6.2E-2</v>
       </c>
       <c r="G235">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>43758273.25</v>
       </c>
-    </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I235">
+        <f t="shared" si="7"/>
+        <v>15888.802</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>20181227</v>
       </c>
@@ -54646,11 +55579,15 @@
         <v>6.1100000000000002E-2</v>
       </c>
       <c r="G236">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>46314413.879999995</v>
       </c>
-    </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I236">
+        <f t="shared" si="7"/>
+        <v>15614.471600000001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>20181228</v>
       </c>
@@ -54667,11 +55604,15 @@
         <v>6.3299999999999995E-2</v>
       </c>
       <c r="G237">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45440346</v>
       </c>
-    </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I237">
+        <f t="shared" si="7"/>
+        <v>16177.580999999998</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>20181229</v>
       </c>
@@ -54688,11 +55629,15 @@
         <v>5.6399999999999999E-2</v>
       </c>
       <c r="G238">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>36726787.75</v>
       </c>
-    </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I238">
+        <f t="shared" si="7"/>
+        <v>12311.3868</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>20181230</v>
       </c>
@@ -54709,11 +55654,15 @@
         <v>5.5300000000000002E-2</v>
       </c>
       <c r="G239">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>36630639</v>
       </c>
-    </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I239">
+        <f t="shared" si="7"/>
+        <v>10846.984400000001</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>20181231</v>
       </c>
@@ -54730,11 +55679,15 @@
         <v>6.3399999999999998E-2</v>
       </c>
       <c r="G240">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>48312847.140000001</v>
       </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I240">
+        <f t="shared" si="7"/>
+        <v>16118.689199999999</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>20190101</v>
       </c>
@@ -54742,11 +55695,15 @@
         <v>0</v>
       </c>
       <c r="G241">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I241">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>20190102</v>
       </c>
@@ -54763,11 +55720,15 @@
         <v>6.2600000000000003E-2</v>
       </c>
       <c r="G242">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>41930372.769999996</v>
       </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I242">
+        <f t="shared" si="7"/>
+        <v>15918.741800000002</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>20190103</v>
       </c>
@@ -54784,11 +55745,15 @@
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="G243">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>46831448.449999996</v>
       </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I243">
+        <f t="shared" si="7"/>
+        <v>16632.928799999998</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>20190104</v>
       </c>
@@ -54805,11 +55770,15 @@
         <v>6.7599999999999993E-2</v>
       </c>
       <c r="G244">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>48731017.280000001</v>
       </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I244">
+        <f t="shared" si="7"/>
+        <v>15294.905599999998</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>20190105</v>
       </c>
@@ -54826,11 +55795,15 @@
         <v>6.1199999999999997E-2</v>
       </c>
       <c r="G245">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45035697.460000001</v>
       </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I245">
+        <f t="shared" si="7"/>
+        <v>13323.913199999999</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>20190106</v>
       </c>
@@ -54847,11 +55820,15 @@
         <v>5.9700000000000003E-2</v>
       </c>
       <c r="G246">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>42891990.600000001</v>
       </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I246">
+        <f t="shared" si="7"/>
+        <v>11927.761500000001</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>20190107</v>
       </c>
@@ -54868,11 +55845,15 @@
         <v>7.2400000000000006E-2</v>
       </c>
       <c r="G247">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>56063525.159999996</v>
       </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I247">
+        <f t="shared" si="7"/>
+        <v>18056.849600000001</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>20190108</v>
       </c>
@@ -54889,11 +55870,15 @@
         <v>8.1900000000000001E-2</v>
       </c>
       <c r="G248">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>60519210.689999998</v>
       </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I248">
+        <f t="shared" si="7"/>
+        <v>20910.953700000002</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>20190109</v>
       </c>
@@ -54910,11 +55895,15 @@
         <v>6.9500000000000006E-2</v>
       </c>
       <c r="G249">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>52958503.350000001</v>
       </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I249">
+        <f t="shared" si="7"/>
+        <v>17691.016500000002</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>20190110</v>
       </c>
@@ -54931,11 +55920,15 @@
         <v>6.6500000000000004E-2</v>
       </c>
       <c r="G250">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>56707125.199999996</v>
       </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I250">
+        <f t="shared" si="7"/>
+        <v>17282.419000000002</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>20190111</v>
       </c>
@@ -54952,11 +55945,15 @@
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="G251">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>63197492.380000003</v>
       </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I251">
+        <f t="shared" si="7"/>
+        <v>19957.645</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>20190112</v>
       </c>
@@ -54973,11 +55970,15 @@
         <v>0.1114</v>
       </c>
       <c r="G252">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>90800463.600000009</v>
       </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I252">
+        <f t="shared" si="7"/>
+        <v>24508.557000000001</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>20190113</v>
       </c>
@@ -54994,11 +55995,15 @@
         <v>6.0400000000000002E-2</v>
       </c>
       <c r="G253">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>42653099.280000001</v>
       </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I253">
+        <f t="shared" si="7"/>
+        <v>12260.837600000001</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>20190114</v>
       </c>
@@ -55015,11 +56020,15 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="G254">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>59202796.5</v>
       </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I254">
+        <f t="shared" si="7"/>
+        <v>19342.194</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>20190115</v>
       </c>
@@ -55036,11 +56045,15 @@
         <v>7.4200000000000002E-2</v>
       </c>
       <c r="G255">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>61459143.199999996</v>
       </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I255">
+        <f t="shared" si="7"/>
+        <v>19245.699199999999</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>20190116</v>
       </c>
@@ -55057,8 +56070,12 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="G256">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>66386109.059999995</v>
+      </c>
+      <c r="I256">
+        <f t="shared" si="7"/>
+        <v>20993.499</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
@@ -55078,8 +56095,12 @@
         <v>7.46E-2</v>
       </c>
       <c r="G257">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>63575346.049999997</v>
+      </c>
+      <c r="I257">
+        <f t="shared" si="7"/>
+        <v>19623.156999999999</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.25">
@@ -55099,8 +56120,12 @@
         <v>8.2299999999999998E-2</v>
       </c>
       <c r="G258">
-        <f t="shared" ref="G258:G270" si="4">D258*C258</f>
+        <f t="shared" ref="G258:G270" si="8">D258*C258</f>
         <v>42889489.600000001</v>
+      </c>
+      <c r="I258">
+        <f t="shared" si="7"/>
+        <v>13487.982399999999</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
@@ -55120,8 +56145,12 @@
         <v>6.3500000000000001E-2</v>
       </c>
       <c r="G259">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>45934073.919999994</v>
+      </c>
+      <c r="I259">
+        <f t="shared" ref="I259:I270" si="9">E259*C259</f>
+        <v>14039.342000000001</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
@@ -55141,8 +56170,12 @@
         <v>9.2899999999999996E-2</v>
       </c>
       <c r="G260">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65970982</v>
+      </c>
+      <c r="I260">
+        <f t="shared" si="9"/>
+        <v>18727.896799999999</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
@@ -55162,8 +56195,12 @@
         <v>7.6300000000000007E-2</v>
       </c>
       <c r="G261">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59421272.219999999</v>
+      </c>
+      <c r="I261">
+        <f t="shared" si="9"/>
+        <v>19786.3449</v>
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.25">
@@ -55183,8 +56220,12 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="G262">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>62835760.640000001</v>
+      </c>
+      <c r="I262">
+        <f t="shared" si="9"/>
+        <v>19533.367999999999</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
@@ -55204,8 +56245,12 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="G263">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>72333381.390000001</v>
+      </c>
+      <c r="I263">
+        <f t="shared" si="9"/>
+        <v>22781.351999999999</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
@@ -55225,8 +56270,12 @@
         <v>9.1200000000000003E-2</v>
       </c>
       <c r="G264">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>78354453.299999997</v>
+      </c>
+      <c r="I264">
+        <f t="shared" si="9"/>
+        <v>23533.430400000001</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
@@ -55246,8 +56295,12 @@
         <v>7.4899999999999994E-2</v>
       </c>
       <c r="G265">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59010802.68</v>
+      </c>
+      <c r="I265">
+        <f t="shared" si="9"/>
+        <v>19322.851799999997</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
@@ -55267,8 +56320,12 @@
         <v>6.6699999999999995E-2</v>
       </c>
       <c r="G266">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48472191.600000001</v>
+      </c>
+      <c r="I266">
+        <f t="shared" si="9"/>
+        <v>15153.2395</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
@@ -55288,8 +56345,12 @@
         <v>5.9499999999999997E-2</v>
       </c>
       <c r="G267">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>39647124</v>
+      </c>
+      <c r="I267">
+        <f t="shared" si="9"/>
+        <v>11914.161</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
@@ -55309,8 +56370,12 @@
         <v>7.8700000000000006E-2</v>
       </c>
       <c r="G268">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>60464568.780000001</v>
+      </c>
+      <c r="I268">
+        <f t="shared" si="9"/>
+        <v>20397.6234</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
@@ -55330,8 +56395,12 @@
         <v>7.3099999999999998E-2</v>
       </c>
       <c r="G269">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>58576636.049999997</v>
+      </c>
+      <c r="I269">
+        <f t="shared" si="9"/>
+        <v>18743.497899999998</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
@@ -55351,8 +56420,12 @@
         <v>5.7799999999999997E-2</v>
       </c>
       <c r="G270">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>42825617.280000001</v>
+      </c>
+      <c r="I270">
+        <f t="shared" si="9"/>
+        <v>15059.4432</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
@@ -55365,8 +56438,42 @@
         <v>17064849071.529999</v>
       </c>
       <c r="I271">
+        <f>SUM(I2:I270)</f>
+        <v>5318005.6041000029</v>
+      </c>
+    </row>
+    <row r="273" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G273">
         <f>G271/C271</f>
         <v>274.20336183413121</v>
+      </c>
+      <c r="I273">
+        <f>I271/C271</f>
+        <v>8.5451386577439573E-2</v>
+      </c>
+      <c r="K273">
+        <f>G273/60</f>
+        <v>4.5700560305688533</v>
+      </c>
+      <c r="M273">
+        <f>I273*100</f>
+        <v>8.5451386577439568</v>
+      </c>
+    </row>
+    <row r="275" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G275">
+        <v>926.68</v>
+      </c>
+      <c r="I275">
+        <v>0.27960000000000002</v>
+      </c>
+      <c r="K275">
+        <f>G275/60</f>
+        <v>15.444666666666667</v>
+      </c>
+      <c r="M275">
+        <f>I275*100</f>
+        <v>27.96</v>
       </c>
     </row>
   </sheetData>
@@ -56437,7 +57544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update overall STD for GTFS version
</commit_message>
<xml_diff>
--- a/doc/APC-GTFS.xlsx
+++ b/doc/APC-GTFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ro2_apc" sheetId="1" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="205">
   <si>
     <t>Date</t>
   </si>
@@ -643,6 +643,15 @@
   </si>
   <si>
     <t>20190130 1034 233705 166.62 0.0638</t>
+  </si>
+  <si>
+    <t>transfer risk average</t>
+  </si>
+  <si>
+    <t>attp average</t>
+  </si>
+  <si>
+    <t>for jan to jan</t>
   </si>
 </sst>
 </file>
@@ -11311,7 +11320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -39860,7 +39869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I271"/>
   <sheetViews>
-    <sheetView topLeftCell="A222" workbookViewId="0">
+    <sheetView topLeftCell="A255" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -45467,9 +45476,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I275"/>
+  <dimension ref="A2:I279"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
       <selection activeCell="H279" sqref="H279"/>
     </sheetView>
   </sheetViews>
@@ -51003,12 +51012,43 @@
         <v>225.84962443626904</v>
       </c>
     </row>
-    <row r="275" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E274" t="s">
+        <v>202</v>
+      </c>
+      <c r="G274" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="275" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C275" t="s">
+        <v>204</v>
+      </c>
       <c r="E275">
         <v>7.1400000000000005E-2</v>
       </c>
       <c r="G275">
         <v>224.36</v>
+      </c>
+    </row>
+    <row r="276" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G276">
+        <f>G275/60</f>
+        <v>3.7393333333333336</v>
+      </c>
+    </row>
+    <row r="278" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E278">
+        <v>0.25750000000000001</v>
+      </c>
+      <c r="G278">
+        <v>778.17</v>
+      </c>
+    </row>
+    <row r="279" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G279">
+        <f>G278/60</f>
+        <v>12.9695</v>
       </c>
     </row>
   </sheetData>
@@ -58312,10 +58352,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I9"/>
+  <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G1:G9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58323,7 +58363,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20180901</v>
       </c>
@@ -58343,8 +58383,12 @@
         <f>D2*C2</f>
         <v>77328597.24000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>E2*C2</f>
+        <v>24469.315200000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20180908</v>
       </c>
@@ -58364,8 +58408,12 @@
         <f t="shared" ref="G3:G8" si="0">D3*C3</f>
         <v>63419802</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="1">E3*C3</f>
+        <v>20575.434400000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20180922</v>
       </c>
@@ -58385,8 +58433,12 @@
         <f t="shared" si="0"/>
         <v>73069294.859999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>23686.376400000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20181006</v>
       </c>
@@ -58406,8 +58458,12 @@
         <f t="shared" si="0"/>
         <v>86870016.280000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>26306.146000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20181013</v>
       </c>
@@ -58427,8 +58483,12 @@
         <f t="shared" si="0"/>
         <v>62189160.120000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>20185.644899999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20181103</v>
       </c>
@@ -58448,8 +58508,12 @@
         <f t="shared" si="0"/>
         <v>71501745</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>23275.852599999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20181124</v>
       </c>
@@ -58469,8 +58533,12 @@
         <f t="shared" si="0"/>
         <v>60192128.780000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>20190.419999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9">
         <f>SUM(C2:C8)</f>
         <v>1604221</v>
@@ -58479,9 +58547,23 @@
         <f>SUM(G2:G8)</f>
         <v>494570744.27999997</v>
       </c>
+      <c r="H9">
+        <f>SUM(H2:H8)</f>
+        <v>158689.18949999998</v>
+      </c>
       <c r="I9">
         <f>G9/C9</f>
         <v>308.2933986526794</v>
+      </c>
+      <c r="J9">
+        <f>H9/C9</f>
+        <v>9.8919780691064371E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f>I9/60</f>
+        <v>5.13822331087799</v>
       </c>
     </row>
   </sheetData>
@@ -58491,10 +58573,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I14"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58502,7 +58584,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20180515</v>
       </c>
@@ -58522,8 +58604,12 @@
         <f>D2*C2</f>
         <v>74493083.280000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>E2*C2</f>
+        <v>21537.2703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20180521</v>
       </c>
@@ -58543,8 +58629,12 @@
         <f>D3*C3</f>
         <v>60662424.100000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="0">E3*C3</f>
+        <v>20269.129499999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20180621</v>
       </c>
@@ -58561,11 +58651,15 @@
         <v>0.1163</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G13" si="0">D4*C4</f>
+        <f t="shared" ref="G4:G13" si="1">D4*C4</f>
         <v>105474051.33999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>30197.760200000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20180720</v>
       </c>
@@ -58582,11 +58676,15 @@
         <v>0.1045</v>
       </c>
       <c r="G5">
+        <f t="shared" si="1"/>
+        <v>87125532.25999999</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>87125532.25999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26638.826499999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20180817</v>
       </c>
@@ -58603,11 +58701,15 @@
         <v>9.7600000000000006E-2</v>
       </c>
       <c r="G6">
+        <f t="shared" si="1"/>
+        <v>82508440.950000003</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>82508440.950000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25439.342400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20180901</v>
       </c>
@@ -58624,11 +58726,15 @@
         <v>0.1056</v>
       </c>
       <c r="G7">
+        <f t="shared" si="1"/>
+        <v>77328597.24000001</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>77328597.24000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24469.315200000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20180908</v>
       </c>
@@ -58645,11 +58751,15 @@
         <v>8.9300000000000004E-2</v>
       </c>
       <c r="G8">
+        <f t="shared" si="1"/>
+        <v>63419802</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>63419802</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20575.434400000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20180909</v>
       </c>
@@ -58666,11 +58776,15 @@
         <v>7.6399999999999996E-2</v>
       </c>
       <c r="G9">
+        <f t="shared" si="1"/>
+        <v>46975095.75</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>46975095.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15224.609999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20180924</v>
       </c>
@@ -58687,11 +58801,15 @@
         <v>9.6799999999999997E-2</v>
       </c>
       <c r="G10">
+        <f t="shared" si="1"/>
+        <v>78292568.200000003</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>78292568.200000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25090.947199999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20181101</v>
       </c>
@@ -58708,11 +58826,15 @@
         <v>9.9099999999999994E-2</v>
       </c>
       <c r="G11">
+        <f t="shared" si="1"/>
+        <v>32487802.739999998</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>32487802.739999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10583.285399999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20181215</v>
       </c>
@@ -58729,11 +58851,15 @@
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="G12">
+        <f t="shared" si="1"/>
+        <v>45909873.899999999</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>45909873.899999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14593.867199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20181231</v>
       </c>
@@ -58750,11 +58876,15 @@
         <v>6.3399999999999998E-2</v>
       </c>
       <c r="G13">
+        <f t="shared" si="1"/>
+        <v>48312847.140000001</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>48312847.140000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16118.689199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>SUM(C2:C13)</f>
         <v>2767882</v>
@@ -58763,9 +58893,23 @@
         <f>SUM(G2:G13)</f>
         <v>802990118.89999998</v>
       </c>
+      <c r="H14">
+        <f>SUM(H2:H13)</f>
+        <v>250738.47749999998</v>
+      </c>
       <c r="I14">
         <f>G14/C14</f>
         <v>290.10995371189955</v>
+      </c>
+      <c r="J14">
+        <f>H14/C14</f>
+        <v>9.0588571875535151E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f>I14/60</f>
+        <v>4.8351658951983261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update GTFS version re-cartography work
</commit_message>
<xml_diff>
--- a/doc/APC-GTFS.xlsx
+++ b/doc/APC-GTFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ro2_apc" sheetId="1" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="205">
   <si>
     <t>Date</t>
   </si>
@@ -643,6 +643,15 @@
   </si>
   <si>
     <t>20190130 1034 233705 166.62 0.0638</t>
+  </si>
+  <si>
+    <t>transfer risk average</t>
+  </si>
+  <si>
+    <t>attp average</t>
+  </si>
+  <si>
+    <t>for jan to jan</t>
   </si>
 </sst>
 </file>
@@ -11311,7 +11320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -39860,7 +39869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I271"/>
   <sheetViews>
-    <sheetView topLeftCell="A222" workbookViewId="0">
+    <sheetView topLeftCell="A255" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -45467,9 +45476,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I275"/>
+  <dimension ref="A2:I279"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
       <selection activeCell="H279" sqref="H279"/>
     </sheetView>
   </sheetViews>
@@ -51003,12 +51012,43 @@
         <v>225.84962443626904</v>
       </c>
     </row>
-    <row r="275" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E274" t="s">
+        <v>202</v>
+      </c>
+      <c r="G274" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="275" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C275" t="s">
+        <v>204</v>
+      </c>
       <c r="E275">
         <v>7.1400000000000005E-2</v>
       </c>
       <c r="G275">
         <v>224.36</v>
+      </c>
+    </row>
+    <row r="276" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G276">
+        <f>G275/60</f>
+        <v>3.7393333333333336</v>
+      </c>
+    </row>
+    <row r="278" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E278">
+        <v>0.25750000000000001</v>
+      </c>
+      <c r="G278">
+        <v>778.17</v>
+      </c>
+    </row>
+    <row r="279" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G279">
+        <f>G278/60</f>
+        <v>12.9695</v>
       </c>
     </row>
   </sheetData>
@@ -58312,10 +58352,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I9"/>
+  <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G1:G9"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58323,7 +58363,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20180901</v>
       </c>
@@ -58343,8 +58383,12 @@
         <f>D2*C2</f>
         <v>77328597.24000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>E2*C2</f>
+        <v>24469.315200000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20180908</v>
       </c>
@@ -58364,8 +58408,12 @@
         <f t="shared" ref="G3:G8" si="0">D3*C3</f>
         <v>63419802</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="1">E3*C3</f>
+        <v>20575.434400000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20180922</v>
       </c>
@@ -58385,8 +58433,12 @@
         <f t="shared" si="0"/>
         <v>73069294.859999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>23686.376400000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20181006</v>
       </c>
@@ -58406,8 +58458,12 @@
         <f t="shared" si="0"/>
         <v>86870016.280000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>26306.146000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20181013</v>
       </c>
@@ -58427,8 +58483,12 @@
         <f t="shared" si="0"/>
         <v>62189160.120000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>20185.644899999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20181103</v>
       </c>
@@ -58448,8 +58508,12 @@
         <f t="shared" si="0"/>
         <v>71501745</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>23275.852599999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20181124</v>
       </c>
@@ -58469,8 +58533,12 @@
         <f t="shared" si="0"/>
         <v>60192128.780000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>20190.419999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9">
         <f>SUM(C2:C8)</f>
         <v>1604221</v>
@@ -58479,9 +58547,23 @@
         <f>SUM(G2:G8)</f>
         <v>494570744.27999997</v>
       </c>
+      <c r="H9">
+        <f>SUM(H2:H8)</f>
+        <v>158689.18949999998</v>
+      </c>
       <c r="I9">
         <f>G9/C9</f>
         <v>308.2933986526794</v>
+      </c>
+      <c r="J9">
+        <f>H9/C9</f>
+        <v>9.8919780691064371E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f>I9/60</f>
+        <v>5.13822331087799</v>
       </c>
     </row>
   </sheetData>
@@ -58491,10 +58573,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I14"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58502,7 +58584,7 @@
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20180515</v>
       </c>
@@ -58522,8 +58604,12 @@
         <f>D2*C2</f>
         <v>74493083.280000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>E2*C2</f>
+        <v>21537.2703</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20180521</v>
       </c>
@@ -58543,8 +58629,12 @@
         <f>D3*C3</f>
         <v>60662424.100000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="0">E3*C3</f>
+        <v>20269.129499999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20180621</v>
       </c>
@@ -58561,11 +58651,15 @@
         <v>0.1163</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G13" si="0">D4*C4</f>
+        <f t="shared" ref="G4:G13" si="1">D4*C4</f>
         <v>105474051.33999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>30197.760200000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20180720</v>
       </c>
@@ -58582,11 +58676,15 @@
         <v>0.1045</v>
       </c>
       <c r="G5">
+        <f t="shared" si="1"/>
+        <v>87125532.25999999</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="0"/>
-        <v>87125532.25999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26638.826499999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20180817</v>
       </c>
@@ -58603,11 +58701,15 @@
         <v>9.7600000000000006E-2</v>
       </c>
       <c r="G6">
+        <f t="shared" si="1"/>
+        <v>82508440.950000003</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>82508440.950000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25439.342400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20180901</v>
       </c>
@@ -58624,11 +58726,15 @@
         <v>0.1056</v>
       </c>
       <c r="G7">
+        <f t="shared" si="1"/>
+        <v>77328597.24000001</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>77328597.24000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24469.315200000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20180908</v>
       </c>
@@ -58645,11 +58751,15 @@
         <v>8.9300000000000004E-2</v>
       </c>
       <c r="G8">
+        <f t="shared" si="1"/>
+        <v>63419802</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>63419802</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20575.434400000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20180909</v>
       </c>
@@ -58666,11 +58776,15 @@
         <v>7.6399999999999996E-2</v>
       </c>
       <c r="G9">
+        <f t="shared" si="1"/>
+        <v>46975095.75</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="0"/>
-        <v>46975095.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15224.609999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20180924</v>
       </c>
@@ -58687,11 +58801,15 @@
         <v>9.6799999999999997E-2</v>
       </c>
       <c r="G10">
+        <f t="shared" si="1"/>
+        <v>78292568.200000003</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="0"/>
-        <v>78292568.200000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25090.947199999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20181101</v>
       </c>
@@ -58708,11 +58826,15 @@
         <v>9.9099999999999994E-2</v>
       </c>
       <c r="G11">
+        <f t="shared" si="1"/>
+        <v>32487802.739999998</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="0"/>
-        <v>32487802.739999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>10583.285399999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20181215</v>
       </c>
@@ -58729,11 +58851,15 @@
         <v>6.4799999999999996E-2</v>
       </c>
       <c r="G12">
+        <f t="shared" si="1"/>
+        <v>45909873.899999999</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>45909873.899999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14593.867199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20181231</v>
       </c>
@@ -58750,11 +58876,15 @@
         <v>6.3399999999999998E-2</v>
       </c>
       <c r="G13">
+        <f t="shared" si="1"/>
+        <v>48312847.140000001</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>48312847.140000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16118.689199999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14">
         <f>SUM(C2:C13)</f>
         <v>2767882</v>
@@ -58763,9 +58893,23 @@
         <f>SUM(G2:G13)</f>
         <v>802990118.89999998</v>
       </c>
+      <c r="H14">
+        <f>SUM(H2:H13)</f>
+        <v>250738.47749999998</v>
+      </c>
       <c r="I14">
         <f>G14/C14</f>
         <v>290.10995371189955</v>
+      </c>
+      <c r="J14">
+        <f>H14/C14</f>
+        <v>9.0588571875535151E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f>I14/60</f>
+        <v>4.8351658951983261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lite version with new added pictures
</commit_message>
<xml_diff>
--- a/doc/APC-GTFS.xlsx
+++ b/doc/APC-GTFS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ro2_apc" sheetId="1" state="hidden" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Average saving time (-2)</t>
+  </si>
+  <si>
+    <t>a_attp</t>
+  </si>
+  <si>
+    <t>b_attp</t>
   </si>
 </sst>
 </file>
@@ -5029,6 +5035,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6917,6 +6924,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18908,14 +18916,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX88"/>
+  <dimension ref="A1:AX93"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AT17" sqref="AT17"/>
+    <sheetView tabSelected="1" topLeftCell="F64" workbookViewId="0">
+      <selection activeCell="AG94" sqref="AG94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32148,6 +32157,122 @@
       <c r="AX88">
         <f t="shared" si="43"/>
         <v>1.0848848814046741</v>
+      </c>
+    </row>
+    <row r="89" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f>SUM(F2:F88)</f>
+        <v>2033208</v>
+      </c>
+      <c r="G89">
+        <f>SUM(G2:G88)</f>
+        <v>1481313</v>
+      </c>
+      <c r="H89">
+        <f>SUM(H2:H88)</f>
+        <v>367013444</v>
+      </c>
+      <c r="I89">
+        <f>SUM(I2:I88)</f>
+        <v>258578936</v>
+      </c>
+      <c r="J89">
+        <f t="shared" ref="J89:K89" si="44">SUM(J2:J88)</f>
+        <v>117365</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="44"/>
+        <v>130319</v>
+      </c>
+      <c r="AB89">
+        <f>SUM(AB2:AB88)</f>
+        <v>2035820</v>
+      </c>
+      <c r="AC89">
+        <f>SUM(AC2:AC88)</f>
+        <v>1479902</v>
+      </c>
+      <c r="AD89">
+        <f>SUM(AD2:AD88)</f>
+        <v>92131481</v>
+      </c>
+      <c r="AE89">
+        <f>SUM(AE2:AE88)</f>
+        <v>229811659</v>
+      </c>
+      <c r="AF89">
+        <f t="shared" ref="AF89" si="45">SUM(AF2:AF88)</f>
+        <v>10612</v>
+      </c>
+      <c r="AG89">
+        <f t="shared" ref="AG89" si="46">SUM(AG2:AG88)</f>
+        <v>263881</v>
+      </c>
+    </row>
+    <row r="91" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="H91">
+        <f>H89/F89</f>
+        <v>180.50954157174277</v>
+      </c>
+      <c r="I91">
+        <f>I89/G89</f>
+        <v>174.56063370806845</v>
+      </c>
+      <c r="J91">
+        <f>J89/F89</f>
+        <v>5.7724049875861203E-2</v>
+      </c>
+      <c r="K91">
+        <f>K89/G89</f>
+        <v>8.797532999440362E-2</v>
+      </c>
+      <c r="AD91">
+        <f>AD89/AB89</f>
+        <v>45.255219518425008</v>
+      </c>
+      <c r="AE91">
+        <f>AE89/AC89</f>
+        <v>155.28843058526849</v>
+      </c>
+      <c r="AF91">
+        <f>AF89/AB89</f>
+        <v>5.2126415891385293E-3</v>
+      </c>
+      <c r="AG91">
+        <f>AG89/AC89</f>
+        <v>0.17830977997191705</v>
+      </c>
+    </row>
+    <row r="92" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AD92" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE92" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF92" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG92" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AD93">
+        <f>(AD91-H91)/60</f>
+        <v>-2.2542387008886293</v>
+      </c>
+      <c r="AE93">
+        <f>(AE91-I91)/60</f>
+        <v>-0.32120338537999943</v>
+      </c>
+      <c r="AF93">
+        <f>(AF91-J91)*100</f>
+        <v>-5.2511408286722672</v>
+      </c>
+      <c r="AG93">
+        <f>(AG91-K91)*100</f>
+        <v>9.0334449977513422</v>
       </c>
     </row>
   </sheetData>
@@ -35605,7 +35730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>

</xml_diff>